<commit_message>
MRD: date format update
</commit_message>
<xml_diff>
--- a/data/r539cy_BLS_Weekly_Jobs_Claims_IN_HenryCo.xlsx
+++ b/data/r539cy_BLS_Weekly_Jobs_Claims_IN_HenryCo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\DataViz\GitHub\Project-2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\DataViz\GitHub\Project-2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1DEBD57-068E-4882-A079-FAA1D8C72AC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424E348B-8639-43A4-A7A5-371FB5AF4937}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{C6E2B8C8-1A64-4933-9E63-C22C685B186D}"/>
   </bookViews>
@@ -83,19 +83,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -413,19 +410,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47BBA864-F7F2-4118-9CC0-97DEE32A8AD2}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -436,7 +435,7 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>43897</v>
       </c>
       <c r="C2" s="1">
@@ -447,7 +446,7 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>43904</v>
       </c>
       <c r="C3" s="1">
@@ -458,7 +457,7 @@
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>43911</v>
       </c>
       <c r="C4" s="1">
@@ -469,7 +468,7 @@
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>43918</v>
       </c>
       <c r="C5" s="1">
@@ -480,7 +479,7 @@
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>43862</v>
       </c>
       <c r="C6" s="1">
@@ -491,7 +490,7 @@
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>43869</v>
       </c>
       <c r="C7" s="1">
@@ -502,7 +501,7 @@
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>43876</v>
       </c>
       <c r="C8" s="1">
@@ -513,7 +512,7 @@
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>43883</v>
       </c>
       <c r="C9" s="1">
@@ -524,7 +523,7 @@
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>43890</v>
       </c>
       <c r="C10" s="1">
@@ -535,7 +534,7 @@
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>43834</v>
       </c>
       <c r="C11" s="1">
@@ -546,7 +545,7 @@
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>43841</v>
       </c>
       <c r="C12" s="1">
@@ -557,7 +556,7 @@
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <v>43848</v>
       </c>
       <c r="C13" s="1">
@@ -568,7 +567,7 @@
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>43855</v>
       </c>
       <c r="C14" s="1">

</xml_diff>